<commit_message>
figuras atualizadas manualmente antes de criar definir a atualização automática
</commit_message>
<xml_diff>
--- a/Data/g10.1.xlsx
+++ b/Data/g10.1.xlsx
@@ -460,13 +460,13 @@
         <v>2012</v>
       </c>
       <c r="B2" t="n">
-        <v>-6.945459866632464</v>
+        <v>-6.943942466780317</v>
       </c>
       <c r="C2" t="n">
-        <v>7.950444133294465</v>
+        <v>7.985561900211491</v>
       </c>
       <c r="D2" t="n">
-        <v>3.556284007633725</v>
+        <v>3.558416437559409</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2013</v>
       </c>
       <c r="B3" t="n">
-        <v>-3.036886126204696</v>
+        <v>-3.033528379010808</v>
       </c>
       <c r="C3" t="n">
-        <v>4.32053098328069</v>
+        <v>4.334264824683731</v>
       </c>
       <c r="D3" t="n">
-        <v>-5.231148880710634</v>
+        <v>-5.228869536197389</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>2014</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2428913365878027</v>
+        <v>-0.2327678074659945</v>
       </c>
       <c r="C4" t="n">
-        <v>4.089514410991879</v>
+        <v>4.101953574790462</v>
       </c>
       <c r="D4" t="n">
-        <v>1.617967204259418</v>
+        <v>1.61910220795054</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>2015</v>
       </c>
       <c r="B5" t="n">
-        <v>1.240228601278837</v>
+        <v>1.249304374546467</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.167284998707752</v>
+        <v>-1.204086634669399</v>
       </c>
       <c r="D5" t="n">
-        <v>8.069838142886532</v>
+        <v>8.070905286572305</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>2016</v>
       </c>
       <c r="B6" t="n">
-        <v>-5.131386207658939</v>
+        <v>-5.140647810975807</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.644730700475063</v>
+        <v>-3.65206940235947</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1803235434287398</v>
+        <v>0.1819403087696347</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>2017</v>
       </c>
       <c r="B7" t="n">
-        <v>-3.396552155841559</v>
+        <v>-3.399975836171742</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5589478740239961</v>
+        <v>0.5772764519954787</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7501023948736973</v>
+        <v>0.7720863564637304</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>2018</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.181803085586088</v>
+        <v>-3.189489044441729</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.093880967492233</v>
+        <v>-1.088355958105625</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.927233180489829</v>
+        <v>-1.90857259036582</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>2019</v>
       </c>
       <c r="B9" t="n">
-        <v>2.966239721912212</v>
+        <v>2.962637469059248</v>
       </c>
       <c r="C9" t="n">
-        <v>1.02962888897391</v>
+        <v>1.03338185358528</v>
       </c>
       <c r="D9" t="n">
-        <v>9.598603239719171</v>
+        <v>9.619155300664595</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>2020</v>
       </c>
       <c r="B10" t="n">
-        <v>-13.96720279275766</v>
+        <v>-13.97437319254418</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.881326808675356</v>
+        <v>-3.916628966280844</v>
       </c>
       <c r="D10" t="n">
-        <v>-12.16332375821054</v>
+        <v>-12.16490384706811</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>2021</v>
       </c>
       <c r="B11" t="n">
-        <v>-11.06887526366901</v>
+        <v>-11.06390641573395</v>
       </c>
       <c r="C11" t="n">
-        <v>15.31299463552325</v>
+        <v>15.37912276036422</v>
       </c>
       <c r="D11" t="n">
-        <v>-14.1200794564396</v>
+        <v>-14.12152573771694</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>2022</v>
       </c>
       <c r="B12" t="n">
-        <v>-4.743353330200073</v>
+        <v>-4.756691349375375</v>
       </c>
       <c r="C12" t="n">
-        <v>14.57313267306115</v>
+        <v>14.54125736551517</v>
       </c>
       <c r="D12" t="n">
-        <v>-12.92492359235758</v>
+        <v>-12.94678802350021</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>2023</v>
       </c>
       <c r="B13" t="n">
-        <v>-6.023626654444081</v>
+        <v>-6.006456415604633</v>
       </c>
       <c r="C13" t="n">
-        <v>7.51362334105854</v>
+        <v>7.559924425551756</v>
       </c>
       <c r="D13" t="n">
-        <v>-7.480404852174571</v>
+        <v>-7.503098588847368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Script 1 - atualização em 2025-09-20 17:07:42Z
</commit_message>
<xml_diff>
--- a/Data/g10.1.xlsx
+++ b/Data/g10.1.xlsx
@@ -460,13 +460,13 @@
         <v>2012</v>
       </c>
       <c r="B2" t="n">
-        <v>-6.943942466780317</v>
+        <v>-6.943213131802861</v>
       </c>
       <c r="C2" t="n">
-        <v>7.985561900211491</v>
+        <v>7.980742702876276</v>
       </c>
       <c r="D2" t="n">
-        <v>3.558416437559409</v>
+        <v>3.559178325481649</v>
       </c>
     </row>
     <row r="3">
@@ -474,13 +474,13 @@
         <v>2013</v>
       </c>
       <c r="B3" t="n">
-        <v>-3.033528379010808</v>
+        <v>-3.033399858582009</v>
       </c>
       <c r="C3" t="n">
-        <v>4.334264824683731</v>
+        <v>4.325288184342346</v>
       </c>
       <c r="D3" t="n">
-        <v>-5.228869536197389</v>
+        <v>-5.228005074708375</v>
       </c>
     </row>
     <row r="4">
@@ -488,13 +488,13 @@
         <v>2014</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.2327678074659945</v>
+        <v>-0.2288600019107689</v>
       </c>
       <c r="C4" t="n">
-        <v>4.101953574790462</v>
+        <v>4.090352838664701</v>
       </c>
       <c r="D4" t="n">
-        <v>1.61910220795054</v>
+        <v>1.61985019946338</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>2015</v>
       </c>
       <c r="B5" t="n">
-        <v>1.249304374546467</v>
+        <v>1.24772536898583</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.204086634669399</v>
+        <v>-1.19499485174599</v>
       </c>
       <c r="D5" t="n">
-        <v>8.070905286572305</v>
+        <v>8.071533547379129</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>2016</v>
       </c>
       <c r="B6" t="n">
-        <v>-5.140647810975807</v>
+        <v>-5.140084324314231</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.65206940235947</v>
+        <v>-3.652084222111918</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1819403087696347</v>
+        <v>0.1774081972812258</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>2017</v>
       </c>
       <c r="B7" t="n">
-        <v>-3.399975836171742</v>
+        <v>-3.397932324802488</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5772764519954787</v>
+        <v>0.583525770808202</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7720863564637304</v>
+        <v>0.7598352624477389</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>2018</v>
       </c>
       <c r="B8" t="n">
-        <v>-3.189489044441729</v>
+        <v>-3.18596839631059</v>
       </c>
       <c r="C8" t="n">
-        <v>-1.088355958105625</v>
+        <v>-1.091482996358195</v>
       </c>
       <c r="D8" t="n">
-        <v>-1.90857259036582</v>
+        <v>-1.922784329967397</v>
       </c>
     </row>
     <row r="9">
@@ -558,13 +558,13 @@
         <v>2019</v>
       </c>
       <c r="B9" t="n">
-        <v>2.962637469059248</v>
+        <v>2.972239650855424</v>
       </c>
       <c r="C9" t="n">
-        <v>1.03338185358528</v>
+        <v>1.038283775507809</v>
       </c>
       <c r="D9" t="n">
-        <v>9.619155300664595</v>
+        <v>9.604857944187906</v>
       </c>
     </row>
     <row r="10">
@@ -572,13 +572,13 @@
         <v>2020</v>
       </c>
       <c r="B10" t="n">
-        <v>-13.97437319254418</v>
+        <v>-13.97255252459051</v>
       </c>
       <c r="C10" t="n">
-        <v>-3.916628966280844</v>
+        <v>-3.906522121507139</v>
       </c>
       <c r="D10" t="n">
-        <v>-12.16490384706811</v>
+        <v>-12.17208917510788</v>
       </c>
     </row>
     <row r="11">
@@ -586,13 +586,13 @@
         <v>2021</v>
       </c>
       <c r="B11" t="n">
-        <v>-11.06390641573395</v>
+        <v>-11.05852305620129</v>
       </c>
       <c r="C11" t="n">
-        <v>15.37912276036422</v>
+        <v>15.38588480891123</v>
       </c>
       <c r="D11" t="n">
-        <v>-14.12152573771694</v>
+        <v>-14.12283002730265</v>
       </c>
     </row>
     <row r="12">
@@ -600,13 +600,13 @@
         <v>2022</v>
       </c>
       <c r="B12" t="n">
-        <v>-4.756691349375375</v>
+        <v>-4.755431186326897</v>
       </c>
       <c r="C12" t="n">
-        <v>14.54125736551517</v>
+        <v>14.56074928380076</v>
       </c>
       <c r="D12" t="n">
-        <v>-12.94678802350021</v>
+        <v>-12.94489690617815</v>
       </c>
     </row>
     <row r="13">
@@ -614,13 +614,13 @@
         <v>2023</v>
       </c>
       <c r="B13" t="n">
-        <v>-6.006456415604633</v>
+        <v>-6.003665244428714</v>
       </c>
       <c r="C13" t="n">
-        <v>7.559924425551756</v>
+        <v>7.569339803891406</v>
       </c>
       <c r="D13" t="n">
-        <v>-7.503098588847368</v>
+        <v>-7.531773508934014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>